<commit_message>
fix: print report peminjaman, format masih jelek
</commit_message>
<xml_diff>
--- a/public/format/format-laporan.xlsx
+++ b/public/format/format-laporan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KEVIN\KULIAH\SMT 6\PKL\pkl\public\format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9FE3C8B-DAE0-40AE-86DD-E38ECC7E7D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90D676B-6AB3-4FBD-AD35-EFFC40BFC3D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0671F42A-EAFE-49F7-B53D-5DD30C7AEE2C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Tikfns</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>Tanggal Dipinjam</t>
+  </si>
+  <si>
+    <t>Tanggal Jatuh Tempo</t>
   </si>
 </sst>
 </file>
@@ -398,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6300549-6D06-41C6-A585-8BCC849728EF}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -410,19 +413,20 @@
     <col min="3" max="3" width="19.36328125" customWidth="1"/>
     <col min="4" max="4" width="15.453125" customWidth="1"/>
     <col min="5" max="5" width="16.6328125" customWidth="1"/>
+    <col min="6" max="6" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -437,6 +441,9 @@
       </c>
       <c r="E4" t="s">
         <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>